<commit_message>
Updated DevTesting_Forecast DMI for the correct flow magnitude (1000, not 1).
</commit_message>
<xml_diff>
--- a/Input Data/DevTesting/DevTesting_IC.avg.xlsx
+++ b/Input Data/DevTesting/DevTesting_IC.avg.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabaker\Projects\Models\MTOM\MTOM_Dir\DevTesting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabaker\Projects\Models\MTOM\MTOM_Dir\Input Data\DevTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="49">
   <si>
     <t>NaN</t>
   </si>
@@ -505,10 +505,10 @@
   <dimension ref="A1:Z412"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="N47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O23" sqref="O23"/>
+      <selection pane="bottomRight" activeCell="W56" sqref="W56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4729,98 +4729,287 @@
         <v>0</v>
       </c>
       <c r="U62">
-        <v>1394895</v>
+        <v>1447499</v>
       </c>
       <c r="V62">
         <v>577939</v>
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A63" s="4"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
+      <c r="A63" s="4">
+        <v>44835</v>
+      </c>
+      <c r="B63" t="s">
+        <v>0</v>
+      </c>
+      <c r="C63" t="s">
+        <v>0</v>
+      </c>
+      <c r="D63" t="s">
+        <v>0</v>
+      </c>
+      <c r="E63" t="s">
+        <v>0</v>
+      </c>
+      <c r="F63" t="s">
+        <v>0</v>
+      </c>
+      <c r="G63" t="s">
+        <v>0</v>
+      </c>
+      <c r="H63" t="s">
+        <v>0</v>
+      </c>
+      <c r="I63" t="s">
+        <v>0</v>
+      </c>
+      <c r="J63" t="s">
+        <v>0</v>
+      </c>
+      <c r="K63" t="s">
+        <v>0</v>
+      </c>
+      <c r="L63" t="s">
+        <v>0</v>
+      </c>
+      <c r="M63" t="s">
+        <v>0</v>
+      </c>
+      <c r="N63" t="s">
+        <v>0</v>
+      </c>
+      <c r="O63" t="s">
+        <v>0</v>
+      </c>
+      <c r="P63" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>0</v>
+      </c>
+      <c r="R63" t="s">
+        <v>0</v>
+      </c>
+      <c r="S63" t="s">
+        <v>0</v>
+      </c>
+      <c r="T63" t="s">
+        <v>0</v>
+      </c>
+      <c r="U63">
+        <v>1447499</v>
+      </c>
+      <c r="V63">
+        <v>554752</v>
+      </c>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A64" s="4"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A65" s="4"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" s="4">
+        <v>44866</v>
+      </c>
+      <c r="B64" t="s">
+        <v>0</v>
+      </c>
+      <c r="C64" t="s">
+        <v>0</v>
+      </c>
+      <c r="D64" t="s">
+        <v>0</v>
+      </c>
+      <c r="E64" t="s">
+        <v>0</v>
+      </c>
+      <c r="F64" t="s">
+        <v>0</v>
+      </c>
+      <c r="G64" t="s">
+        <v>0</v>
+      </c>
+      <c r="H64" t="s">
+        <v>0</v>
+      </c>
+      <c r="I64" t="s">
+        <v>0</v>
+      </c>
+      <c r="J64" t="s">
+        <v>0</v>
+      </c>
+      <c r="K64" t="s">
+        <v>0</v>
+      </c>
+      <c r="L64" t="s">
+        <v>0</v>
+      </c>
+      <c r="M64" t="s">
+        <v>0</v>
+      </c>
+      <c r="N64" t="s">
+        <v>0</v>
+      </c>
+      <c r="O64" t="s">
+        <v>0</v>
+      </c>
+      <c r="P64" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>0</v>
+      </c>
+      <c r="R64" t="s">
+        <v>0</v>
+      </c>
+      <c r="S64" t="s">
+        <v>0</v>
+      </c>
+      <c r="T64" t="s">
+        <v>0</v>
+      </c>
+      <c r="U64">
+        <v>1409811</v>
+      </c>
+      <c r="V64">
+        <v>566285</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A65" s="4">
+        <v>44896</v>
+      </c>
+      <c r="B65" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65" t="s">
+        <v>0</v>
+      </c>
+      <c r="D65" t="s">
+        <v>0</v>
+      </c>
+      <c r="E65" t="s">
+        <v>0</v>
+      </c>
+      <c r="F65" t="s">
+        <v>0</v>
+      </c>
+      <c r="G65" t="s">
+        <v>0</v>
+      </c>
+      <c r="H65" t="s">
+        <v>0</v>
+      </c>
+      <c r="I65" t="s">
+        <v>0</v>
+      </c>
+      <c r="J65" t="s">
+        <v>0</v>
+      </c>
+      <c r="K65" t="s">
+        <v>0</v>
+      </c>
+      <c r="L65" t="s">
+        <v>0</v>
+      </c>
+      <c r="M65" t="s">
+        <v>0</v>
+      </c>
+      <c r="N65" t="s">
+        <v>0</v>
+      </c>
+      <c r="O65" t="s">
+        <v>0</v>
+      </c>
+      <c r="P65" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>0</v>
+      </c>
+      <c r="R65" t="s">
+        <v>0</v>
+      </c>
+      <c r="S65" t="s">
+        <v>0</v>
+      </c>
+      <c r="T65" t="s">
+        <v>0</v>
+      </c>
+      <c r="U65">
+        <v>1409811</v>
+      </c>
+      <c r="V65">
+        <v>586291</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A66" s="4"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A67" s="4"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A68" s="4"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A69" s="4"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A70" s="4"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A71" s="4"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A72" s="4"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A73" s="4"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A74" s="4"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A75" s="4"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A76" s="4"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A77" s="4"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A78" s="4"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A79" s="4"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A80" s="4"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>

</xml_diff>

<commit_message>
Updated the dates in the excel workbook to match the RiverSMART Run Range.
</commit_message>
<xml_diff>
--- a/Input Data/DevTesting/DevTesting_IC.avg.xlsx
+++ b/Input Data/DevTesting/DevTesting_IC.avg.xlsx
@@ -505,10 +505,10 @@
   <dimension ref="A1:Z412"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="N47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W56" sqref="W56"/>
+      <selection pane="bottomRight" activeCell="C18" sqref="B18:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -589,7 +589,7 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
-        <v>42979</v>
+        <v>43344</v>
       </c>
       <c r="B2" s="1">
         <v>7479.81</v>
@@ -657,7 +657,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
-        <v>43009</v>
+        <v>43374</v>
       </c>
       <c r="B3" s="1">
         <v>7478.29</v>
@@ -725,7 +725,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
-        <v>43040</v>
+        <v>43405</v>
       </c>
       <c r="B4" s="1">
         <v>7477.6</v>
@@ -793,7 +793,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
-        <v>43070</v>
+        <v>43435</v>
       </c>
       <c r="B5" s="1">
         <v>7475.84</v>
@@ -861,7 +861,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B6" s="1">
         <v>7473.49</v>
@@ -929,7 +929,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
-        <v>43132</v>
+        <v>43497</v>
       </c>
       <c r="B7" s="1">
         <v>7491.67</v>
@@ -997,7 +997,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
-        <v>43160</v>
+        <v>43525</v>
       </c>
       <c r="B8" s="1">
         <v>7501.51</v>
@@ -1065,7 +1065,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
-        <v>43191</v>
+        <v>43556</v>
       </c>
       <c r="B9" s="1">
         <v>7499.99</v>
@@ -1133,7 +1133,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
-        <v>43221</v>
+        <v>43586</v>
       </c>
       <c r="B10" s="1">
         <v>7497.56</v>
@@ -1201,7 +1201,7 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
-        <v>43252</v>
+        <v>43617</v>
       </c>
       <c r="B11" s="1">
         <v>7492.05</v>
@@ -1269,7 +1269,7 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
-        <v>43282</v>
+        <v>43647</v>
       </c>
       <c r="B12" s="1">
         <v>7486.61</v>
@@ -1337,7 +1337,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
-        <v>43313</v>
+        <v>43678</v>
       </c>
       <c r="B13" s="1">
         <v>7485.87</v>
@@ -1405,7 +1405,7 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
-        <v>43344</v>
+        <v>43709</v>
       </c>
       <c r="B14" s="1">
         <v>7485.06</v>
@@ -1473,7 +1473,7 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
-        <v>43374</v>
+        <v>43739</v>
       </c>
       <c r="B15" s="1">
         <v>7483.65</v>
@@ -1541,7 +1541,7 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
-        <v>43405</v>
+        <v>43770</v>
       </c>
       <c r="B16" s="1">
         <v>7482.23</v>
@@ -1609,7 +1609,7 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
-        <v>43435</v>
+        <v>43800</v>
       </c>
       <c r="B17" s="1">
         <v>7480.99</v>
@@ -1677,7 +1677,7 @@
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B18" s="1">
         <v>7479.65</v>
@@ -1745,7 +1745,7 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
-        <v>43497</v>
+        <v>43862</v>
       </c>
       <c r="B19" s="1">
         <v>7476.52</v>
@@ -1813,7 +1813,7 @@
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
-        <v>43525</v>
+        <v>43891</v>
       </c>
       <c r="B20" s="1">
         <v>7471.79</v>
@@ -1881,7 +1881,7 @@
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
-        <v>43556</v>
+        <v>43922</v>
       </c>
       <c r="B21" s="1">
         <v>7460.33</v>
@@ -1949,7 +1949,7 @@
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
-        <v>43586</v>
+        <v>43952</v>
       </c>
       <c r="B22" s="1">
         <v>7450.91</v>
@@ -2017,7 +2017,7 @@
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
-        <v>43617</v>
+        <v>43983</v>
       </c>
       <c r="B23" s="1">
         <v>7442.66</v>
@@ -2085,7 +2085,7 @@
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
-        <v>43647</v>
+        <v>44013</v>
       </c>
       <c r="B24" s="1">
         <v>7441.48</v>
@@ -2153,7 +2153,7 @@
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A25" s="4">
-        <v>43678</v>
+        <v>44044</v>
       </c>
       <c r="B25" s="1">
         <v>7443.54</v>
@@ -2221,7 +2221,7 @@
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
-        <v>43709</v>
+        <v>44075</v>
       </c>
       <c r="B26" s="1">
         <v>7444.59</v>
@@ -2289,7 +2289,7 @@
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
-        <v>43739</v>
+        <v>44105</v>
       </c>
       <c r="B27" t="s">
         <v>0</v>
@@ -2357,7 +2357,7 @@
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
-        <v>43770</v>
+        <v>44136</v>
       </c>
       <c r="B28" t="s">
         <v>0</v>
@@ -2425,7 +2425,7 @@
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
-        <v>43800</v>
+        <v>44166</v>
       </c>
       <c r="B29" t="s">
         <v>0</v>
@@ -2493,7 +2493,7 @@
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A30" s="4">
-        <v>43831</v>
+        <v>44197</v>
       </c>
       <c r="B30" t="s">
         <v>0</v>
@@ -2561,7 +2561,7 @@
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
-        <v>43862</v>
+        <v>44228</v>
       </c>
       <c r="B31" t="s">
         <v>0</v>
@@ -2629,7 +2629,7 @@
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
-        <v>43891</v>
+        <v>44256</v>
       </c>
       <c r="B32" t="s">
         <v>0</v>
@@ -2697,7 +2697,7 @@
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A33" s="4">
-        <v>43922</v>
+        <v>44287</v>
       </c>
       <c r="B33" t="s">
         <v>0</v>
@@ -2765,7 +2765,7 @@
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A34" s="4">
-        <v>43952</v>
+        <v>44317</v>
       </c>
       <c r="B34" t="s">
         <v>0</v>
@@ -2833,7 +2833,7 @@
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A35" s="4">
-        <v>43983</v>
+        <v>44348</v>
       </c>
       <c r="B35" t="s">
         <v>0</v>
@@ -2901,7 +2901,7 @@
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A36" s="4">
-        <v>44013</v>
+        <v>44378</v>
       </c>
       <c r="B36" t="s">
         <v>0</v>
@@ -2969,7 +2969,7 @@
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A37" s="4">
-        <v>44044</v>
+        <v>44409</v>
       </c>
       <c r="B37" t="s">
         <v>0</v>
@@ -3037,7 +3037,7 @@
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A38" s="4">
-        <v>44075</v>
+        <v>44440</v>
       </c>
       <c r="B38" t="s">
         <v>0</v>
@@ -3105,7 +3105,7 @@
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A39" s="4">
-        <v>44105</v>
+        <v>44470</v>
       </c>
       <c r="B39" t="s">
         <v>0</v>
@@ -3173,7 +3173,7 @@
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A40" s="4">
-        <v>44136</v>
+        <v>44501</v>
       </c>
       <c r="B40" t="s">
         <v>0</v>
@@ -3241,7 +3241,7 @@
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A41" s="4">
-        <v>44166</v>
+        <v>44531</v>
       </c>
       <c r="B41" t="s">
         <v>0</v>
@@ -3309,7 +3309,7 @@
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A42" s="4">
-        <v>44197</v>
+        <v>44562</v>
       </c>
       <c r="B42" t="s">
         <v>0</v>
@@ -3377,7 +3377,7 @@
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A43" s="4">
-        <v>44228</v>
+        <v>44593</v>
       </c>
       <c r="B43" t="s">
         <v>0</v>
@@ -3445,7 +3445,7 @@
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A44" s="4">
-        <v>44256</v>
+        <v>44621</v>
       </c>
       <c r="B44" t="s">
         <v>0</v>
@@ -3513,7 +3513,7 @@
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A45" s="4">
-        <v>44287</v>
+        <v>44652</v>
       </c>
       <c r="B45" t="s">
         <v>0</v>
@@ -3581,7 +3581,7 @@
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A46" s="4">
-        <v>44317</v>
+        <v>44682</v>
       </c>
       <c r="B46" t="s">
         <v>0</v>
@@ -3649,7 +3649,7 @@
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A47" s="4">
-        <v>44348</v>
+        <v>44713</v>
       </c>
       <c r="B47" t="s">
         <v>0</v>
@@ -3717,7 +3717,7 @@
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A48" s="4">
-        <v>44378</v>
+        <v>44743</v>
       </c>
       <c r="B48" t="s">
         <v>0</v>
@@ -3785,7 +3785,7 @@
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A49" s="4">
-        <v>44409</v>
+        <v>44774</v>
       </c>
       <c r="B49" t="s">
         <v>0</v>
@@ -3853,7 +3853,7 @@
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A50" s="4">
-        <v>44440</v>
+        <v>44805</v>
       </c>
       <c r="B50" t="s">
         <v>0</v>
@@ -3921,7 +3921,7 @@
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A51" s="4">
-        <v>44470</v>
+        <v>44835</v>
       </c>
       <c r="B51" t="s">
         <v>0</v>
@@ -3989,7 +3989,7 @@
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A52" s="4">
-        <v>44501</v>
+        <v>44866</v>
       </c>
       <c r="B52" t="s">
         <v>0</v>
@@ -4057,7 +4057,7 @@
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A53" s="4">
-        <v>44531</v>
+        <v>44896</v>
       </c>
       <c r="B53" t="s">
         <v>0</v>
@@ -4125,7 +4125,7 @@
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A54" s="4">
-        <v>44562</v>
+        <v>44927</v>
       </c>
       <c r="B54" t="s">
         <v>0</v>
@@ -4193,7 +4193,7 @@
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A55" s="4">
-        <v>44593</v>
+        <v>44958</v>
       </c>
       <c r="B55" t="s">
         <v>0</v>
@@ -4261,7 +4261,7 @@
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A56" s="4">
-        <v>44621</v>
+        <v>44986</v>
       </c>
       <c r="B56" t="s">
         <v>0</v>
@@ -4329,7 +4329,7 @@
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A57" s="4">
-        <v>44652</v>
+        <v>45017</v>
       </c>
       <c r="B57" t="s">
         <v>0</v>
@@ -4397,7 +4397,7 @@
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A58" s="4">
-        <v>44682</v>
+        <v>45047</v>
       </c>
       <c r="B58" t="s">
         <v>0</v>
@@ -4465,7 +4465,7 @@
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A59" s="4">
-        <v>44713</v>
+        <v>45078</v>
       </c>
       <c r="B59" t="s">
         <v>0</v>
@@ -4533,7 +4533,7 @@
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A60" s="4">
-        <v>44743</v>
+        <v>45108</v>
       </c>
       <c r="B60" t="s">
         <v>0</v>
@@ -4601,7 +4601,7 @@
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A61" s="4">
-        <v>44774</v>
+        <v>45139</v>
       </c>
       <c r="B61" t="s">
         <v>0</v>
@@ -4669,7 +4669,7 @@
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A62" s="4">
-        <v>44805</v>
+        <v>45170</v>
       </c>
       <c r="B62" t="s">
         <v>0</v>
@@ -4737,7 +4737,7 @@
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A63" s="4">
-        <v>44835</v>
+        <v>45200</v>
       </c>
       <c r="B63" t="s">
         <v>0</v>
@@ -4805,7 +4805,7 @@
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A64" s="4">
-        <v>44866</v>
+        <v>45231</v>
       </c>
       <c r="B64" t="s">
         <v>0</v>
@@ -4873,7 +4873,7 @@
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A65" s="4">
-        <v>44896</v>
+        <v>45261</v>
       </c>
       <c r="B65" t="s">
         <v>0</v>
@@ -11582,7 +11582,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11616,7 +11616,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
-        <v>42736</v>
+        <v>43101</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -11639,7 +11639,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -11662,7 +11662,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -11685,7 +11685,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
-        <v>43831</v>
+        <v>44197</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -11708,7 +11708,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
-        <v>44197</v>
+        <v>44562</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
@@ -11740,7 +11740,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11792,7 +11792,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
-        <v>42979</v>
+        <v>43344</v>
       </c>
       <c r="B2" s="1">
         <v>56574.26</v>
@@ -11833,7 +11833,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
-        <v>43009</v>
+        <v>43374</v>
       </c>
       <c r="B3" s="1">
         <v>48231.37</v>
@@ -11874,7 +11874,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
-        <v>43040</v>
+        <v>43405</v>
       </c>
       <c r="B4" s="1">
         <v>33048.080000000002</v>
@@ -11915,7 +11915,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
-        <v>43070</v>
+        <v>43435</v>
       </c>
       <c r="B5" s="1">
         <v>24865.08</v>
@@ -11956,7 +11956,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B6" s="1">
         <v>22252.33</v>
@@ -11997,7 +11997,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
-        <v>43132</v>
+        <v>43497</v>
       </c>
       <c r="B7" s="1">
         <v>22672.799999999999</v>
@@ -12038,7 +12038,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
-        <v>43160</v>
+        <v>43525</v>
       </c>
       <c r="B8" s="1">
         <v>32409.31</v>
@@ -12079,7 +12079,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
-        <v>43191</v>
+        <v>43556</v>
       </c>
       <c r="B9" s="1">
         <v>129304.1</v>
@@ -12120,7 +12120,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
-        <v>43221</v>
+        <v>43586</v>
       </c>
       <c r="B10" s="1">
         <v>242113.9</v>
@@ -12161,7 +12161,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
-        <v>43252</v>
+        <v>43617</v>
       </c>
       <c r="B11" s="1">
         <v>360639</v>
@@ -12202,7 +12202,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
-        <v>43282</v>
+        <v>43647</v>
       </c>
       <c r="B12" s="1">
         <v>117138</v>
@@ -12243,7 +12243,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
-        <v>43313</v>
+        <v>43678</v>
       </c>
       <c r="B13" s="1">
         <v>63574.64</v>
@@ -12284,7 +12284,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
-        <v>43344</v>
+        <v>43709</v>
       </c>
       <c r="B14" s="1">
         <v>48335.02</v>
@@ -12325,7 +12325,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
-        <v>43374</v>
+        <v>43739</v>
       </c>
       <c r="B15" s="1">
         <v>54591.56</v>
@@ -12366,7 +12366,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
-        <v>43405</v>
+        <v>43770</v>
       </c>
       <c r="B16" s="1">
         <v>36683.29</v>
@@ -12407,7 +12407,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
-        <v>43435</v>
+        <v>43800</v>
       </c>
       <c r="B17" s="1">
         <v>33647.79</v>
@@ -12448,7 +12448,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B18" s="1">
         <v>29553.7</v>
@@ -12489,7 +12489,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
-        <v>43497</v>
+        <v>43862</v>
       </c>
       <c r="B19" s="1">
         <v>28053.19</v>
@@ -12530,7 +12530,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
-        <v>43525</v>
+        <v>43891</v>
       </c>
       <c r="B20" s="1">
         <v>53513.79</v>
@@ -12571,7 +12571,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
-        <v>43556</v>
+        <v>43922</v>
       </c>
       <c r="B21" s="1">
         <v>73052.039999999994</v>
@@ -12612,7 +12612,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
-        <v>43586</v>
+        <v>43952</v>
       </c>
       <c r="B22" s="1">
         <v>136242.70000000001</v>
@@ -12653,7 +12653,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
-        <v>43617</v>
+        <v>43983</v>
       </c>
       <c r="B23" s="1">
         <v>367781.3</v>
@@ -12694,7 +12694,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
-        <v>43647</v>
+        <v>44013</v>
       </c>
       <c r="B24" s="1">
         <v>131207.9</v>
@@ -12735,7 +12735,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="4">
-        <v>43678</v>
+        <v>44044</v>
       </c>
       <c r="B25" s="1">
         <v>59293.96</v>
@@ -12776,7 +12776,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
-        <v>43709</v>
+        <v>44075</v>
       </c>
       <c r="B26" s="1">
         <v>38688.67</v>
@@ -12817,7 +12817,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
-        <v>43739</v>
+        <v>44105</v>
       </c>
       <c r="B27" s="1">
         <v>33341.449999999997</v>
@@ -12958,7 +12958,7 @@
   <dimension ref="A1:Z570"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13002,7 +13002,7 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
-        <v>42979</v>
+        <v>43344</v>
       </c>
       <c r="B2" s="1">
         <v>-5894.69</v>
@@ -13045,7 +13045,7 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
-        <v>43009</v>
+        <v>43374</v>
       </c>
       <c r="B3" s="1">
         <v>9566.43</v>
@@ -13092,7 +13092,7 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
-        <v>43040</v>
+        <v>43405</v>
       </c>
       <c r="B4" s="1">
         <v>-5666.19</v>
@@ -13135,7 +13135,7 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
-        <v>43070</v>
+        <v>43435</v>
       </c>
       <c r="B5" s="1">
         <v>-1670.61</v>
@@ -13178,7 +13178,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B6" s="1">
         <v>-21864.400000000001</v>
@@ -13221,7 +13221,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
-        <v>43132</v>
+        <v>43497</v>
       </c>
       <c r="B7" s="1">
         <v>-7545.24</v>
@@ -13264,7 +13264,7 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
-        <v>43160</v>
+        <v>43525</v>
       </c>
       <c r="B8" s="1">
         <v>-21530.83</v>
@@ -13307,7 +13307,7 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
-        <v>43191</v>
+        <v>43556</v>
       </c>
       <c r="B9" s="1">
         <v>-18509.3</v>
@@ -13350,7 +13350,7 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
-        <v>43221</v>
+        <v>43586</v>
       </c>
       <c r="B10" s="1">
         <v>-10435.120000000001</v>
@@ -13393,7 +13393,7 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
-        <v>43252</v>
+        <v>43617</v>
       </c>
       <c r="B11" s="1">
         <v>-18403.490000000002</v>
@@ -13436,7 +13436,7 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
-        <v>43282</v>
+        <v>43647</v>
       </c>
       <c r="B12" s="1">
         <v>-13568.73</v>
@@ -13479,7 +13479,7 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
-        <v>43313</v>
+        <v>43678</v>
       </c>
       <c r="B13" s="1">
         <v>-16631.419999999998</v>
@@ -13522,7 +13522,7 @@
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
-        <v>43344</v>
+        <v>43709</v>
       </c>
       <c r="B14" s="1">
         <v>-16038.95</v>
@@ -13565,7 +13565,7 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
-        <v>43374</v>
+        <v>43739</v>
       </c>
       <c r="B15" s="1">
         <v>-7345.29</v>
@@ -13612,7 +13612,7 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
-        <v>43405</v>
+        <v>43770</v>
       </c>
       <c r="B16" s="1">
         <v>-13474.74</v>
@@ -13655,7 +13655,7 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
-        <v>43435</v>
+        <v>43800</v>
       </c>
       <c r="B17" s="1">
         <v>-12944.09</v>
@@ -13698,7 +13698,7 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B18" s="1">
         <v>-31790.57</v>
@@ -13740,7 +13740,7 @@
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
-        <v>43497</v>
+        <v>43862</v>
       </c>
       <c r="B19" s="1">
         <v>-20499.46</v>
@@ -13783,7 +13783,7 @@
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
-        <v>43525</v>
+        <v>43891</v>
       </c>
       <c r="B20" s="1">
         <v>-15448.75</v>
@@ -13826,7 +13826,7 @@
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
-        <v>43556</v>
+        <v>43922</v>
       </c>
       <c r="B21" s="1">
         <v>-17709.400000000001</v>
@@ -13869,7 +13869,7 @@
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
-        <v>43586</v>
+        <v>43952</v>
       </c>
       <c r="B22" s="1">
         <v>-5794.55</v>
@@ -13913,7 +13913,7 @@
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
-        <v>43617</v>
+        <v>43983</v>
       </c>
       <c r="B23" s="1">
         <v>-15855.95</v>
@@ -13957,7 +13957,7 @@
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
-        <v>43647</v>
+        <v>44013</v>
       </c>
       <c r="B24" s="1">
         <v>-23911.19</v>
@@ -14001,7 +14001,7 @@
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A25" s="4">
-        <v>43678</v>
+        <v>44044</v>
       </c>
       <c r="B25" s="1">
         <v>-11929.89</v>
@@ -14045,7 +14045,7 @@
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
-        <v>43709</v>
+        <v>44075</v>
       </c>
       <c r="B26" s="1">
         <v>-17913.939999999999</v>
@@ -14089,7 +14089,7 @@
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
-        <v>43739</v>
+        <v>44105</v>
       </c>
       <c r="B27" s="1">
         <v>-6785.6</v>
@@ -14137,7 +14137,7 @@
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
-        <v>43770</v>
+        <v>44136</v>
       </c>
       <c r="B28" s="1">
         <v>-29191.95</v>
@@ -14181,7 +14181,7 @@
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
-        <v>43800</v>
+        <v>44166</v>
       </c>
       <c r="B29" s="1">
         <v>-17534.43</v>
@@ -14225,7 +14225,7 @@
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A30" s="4">
-        <v>43831</v>
+        <v>44197</v>
       </c>
       <c r="B30" s="1">
         <v>-23340</v>
@@ -14269,7 +14269,7 @@
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
-        <v>43862</v>
+        <v>44228</v>
       </c>
       <c r="B31" s="1">
         <v>-13790</v>
@@ -14313,7 +14313,7 @@
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
-        <v>43891</v>
+        <v>44256</v>
       </c>
       <c r="B32" s="1">
         <v>-15540</v>
@@ -14357,7 +14357,7 @@
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A33" s="4">
-        <v>43922</v>
+        <v>44287</v>
       </c>
       <c r="B33" s="1">
         <v>-19260</v>
@@ -14401,7 +14401,7 @@
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A34" s="4">
-        <v>43952</v>
+        <v>44317</v>
       </c>
       <c r="B34" s="1">
         <v>-13340</v>
@@ -14445,7 +14445,7 @@
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A35" s="4">
-        <v>43983</v>
+        <v>44348</v>
       </c>
       <c r="B35" s="1">
         <v>-16340</v>
@@ -14489,7 +14489,7 @@
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A36" s="4">
-        <v>44013</v>
+        <v>44378</v>
       </c>
       <c r="B36" s="1">
         <v>-13320</v>
@@ -14533,7 +14533,7 @@
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A37" s="4">
-        <v>44044</v>
+        <v>44409</v>
       </c>
       <c r="B37" s="1">
         <v>-11130</v>
@@ -14577,7 +14577,7 @@
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A38" s="4">
-        <v>44075</v>
+        <v>44440</v>
       </c>
       <c r="B38" s="1">
         <v>-8790</v>
@@ -14621,7 +14621,7 @@
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A39" s="4">
-        <v>44105</v>
+        <v>44470</v>
       </c>
       <c r="B39" s="1">
         <v>-1280</v>
@@ -14669,7 +14669,7 @@
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A40" s="4">
-        <v>44136</v>
+        <v>44501</v>
       </c>
       <c r="B40" s="1">
         <v>-7570</v>
@@ -14713,7 +14713,7 @@
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A41" s="4">
-        <v>44166</v>
+        <v>44531</v>
       </c>
       <c r="B41" s="1">
         <v>-11820</v>
@@ -14757,7 +14757,7 @@
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A42" s="4">
-        <v>44197</v>
+        <v>44562</v>
       </c>
       <c r="B42" s="1">
         <v>-14160</v>
@@ -14801,7 +14801,7 @@
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A43" s="4">
-        <v>44228</v>
+        <v>44593</v>
       </c>
       <c r="B43" s="1">
         <v>-13790</v>
@@ -14845,7 +14845,7 @@
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A44" s="4">
-        <v>44256</v>
+        <v>44621</v>
       </c>
       <c r="B44" s="1">
         <v>-15540</v>
@@ -14889,7 +14889,7 @@
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A45" s="4">
-        <v>44287</v>
+        <v>44652</v>
       </c>
       <c r="B45" s="1">
         <v>-19260</v>
@@ -14933,7 +14933,7 @@
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A46" s="4">
-        <v>44317</v>
+        <v>44682</v>
       </c>
       <c r="B46" s="1">
         <v>-13340</v>
@@ -14977,7 +14977,7 @@
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A47" s="4">
-        <v>44348</v>
+        <v>44713</v>
       </c>
       <c r="B47" s="1">
         <v>-16340</v>
@@ -15021,7 +15021,7 @@
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A48" s="4">
-        <v>44378</v>
+        <v>44743</v>
       </c>
       <c r="B48" s="1">
         <v>-13320</v>
@@ -15065,7 +15065,7 @@
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A49" s="4">
-        <v>44409</v>
+        <v>44774</v>
       </c>
       <c r="B49" s="1">
         <v>-11130</v>
@@ -15109,7 +15109,7 @@
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A50" s="4">
-        <v>44440</v>
+        <v>44805</v>
       </c>
       <c r="B50" s="1">
         <v>-8790</v>
@@ -15153,7 +15153,7 @@
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A51" s="4">
-        <v>44470</v>
+        <v>44835</v>
       </c>
       <c r="B51" s="1">
         <v>-1280</v>
@@ -15200,7 +15200,7 @@
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A52" s="4">
-        <v>44501</v>
+        <v>44866</v>
       </c>
       <c r="B52" s="1">
         <v>-7570</v>
@@ -15243,7 +15243,7 @@
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A53" s="4">
-        <v>44531</v>
+        <v>44896</v>
       </c>
       <c r="B53" s="1">
         <v>-11820</v>
@@ -15286,7 +15286,7 @@
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A54" s="4">
-        <v>44562</v>
+        <v>44927</v>
       </c>
       <c r="B54" s="1">
         <v>-14160</v>
@@ -15329,7 +15329,7 @@
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A55" s="4">
-        <v>44593</v>
+        <v>44958</v>
       </c>
       <c r="B55" s="1">
         <v>-13790</v>
@@ -15373,7 +15373,7 @@
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A56" s="4">
-        <v>44621</v>
+        <v>44986</v>
       </c>
       <c r="B56" s="1">
         <v>-15540</v>
@@ -15417,7 +15417,7 @@
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A57" s="4">
-        <v>44652</v>
+        <v>45017</v>
       </c>
       <c r="B57" s="1">
         <v>-19260</v>
@@ -15461,7 +15461,7 @@
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A58" s="4">
-        <v>44682</v>
+        <v>45047</v>
       </c>
       <c r="B58" s="1">
         <v>-13340</v>
@@ -15505,7 +15505,7 @@
     </row>
     <row r="59" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A59" s="4">
-        <v>44713</v>
+        <v>45078</v>
       </c>
       <c r="B59" s="1">
         <v>-16340</v>
@@ -15549,7 +15549,7 @@
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A60" s="4">
-        <v>44743</v>
+        <v>45108</v>
       </c>
       <c r="B60" s="1">
         <v>10577.18</v>
@@ -15593,7 +15593,7 @@
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A61" s="4">
-        <v>44774</v>
+        <v>45139</v>
       </c>
       <c r="B61" s="1">
         <v>47366.78</v>
@@ -15637,7 +15637,7 @@
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A62" s="4">
-        <v>44805</v>
+        <v>45170</v>
       </c>
       <c r="B62" s="1">
         <v>21405.07</v>

</xml_diff>

<commit_message>
added another year to coor ops in IC spreadsheet.
</commit_message>
<xml_diff>
--- a/Input Data/DevTesting/DevTesting_IC.avg.xlsx
+++ b/Input Data/DevTesting/DevTesting_IC.avg.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Reservoirs" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="49">
   <si>
     <t>NaN</t>
   </si>
@@ -504,11 +504,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z412"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C18" sqref="B18:C18"/>
+      <selection pane="bottomRight" activeCell="K14" sqref="K14:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11581,8 +11581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11700,34 +11700,14 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>3602.46</v>
+        <v>3601</v>
       </c>
       <c r="G5">
-        <v>1082.33</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="4">
-        <v>44562</v>
-      </c>
-      <c r="B6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>3602.46</v>
-      </c>
-      <c r="G6">
-        <v>1082.33</v>
-      </c>
+      <c r="A6" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Model: edit initialization ruleset to fire for development testing tool
Edited execution constraints to fire for development testing tool.
Edited IC to include release tier inputs. Made one Vallecito PE lower so model didnt fail b/c it couldnt release enough since there was such a low initial PE.
</commit_message>
<xml_diff>
--- a/Input Data/DevTesting/DevTesting_IC.avg.xlsx
+++ b/Input Data/DevTesting/DevTesting_IC.avg.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Reservoirs" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="50">
   <si>
     <t>NaN</t>
   </si>
@@ -508,11 +508,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA412"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T1" sqref="T1"/>
+      <selection pane="bottomRight" activeCell="K17" sqref="G17:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12104,8 +12104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:XFD30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12187,11 +12187,11 @@
       <c r="A4" s="4">
         <v>43831</v>
       </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
+      <c r="B4">
+        <v>1.4</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -12210,11 +12210,11 @@
       <c r="A5" s="4">
         <v>44197</v>
       </c>
-      <c r="B5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>0</v>
+      <c r="B5">
+        <v>1.4</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Rule edit: Mead Flood Control Release
Add constraint within IF statement to check if Mead.Outflow is greater than 0  (non-negative) this rule was setting Mead outflow during very low scenarios in which flood control rules should not be executing.

Excel IC file edits - added TARV
The IC files were updated to include a TARV for 2020 which was needed for simulations starting in August and September.
</commit_message>
<xml_diff>
--- a/Input Data/DevTesting/DevTesting_IC.avg.xlsx
+++ b/Input Data/DevTesting/DevTesting_IC.avg.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="50">
   <si>
     <t>NaN</t>
   </si>
@@ -509,10 +509,10 @@
   <dimension ref="A1:AA412"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K17" sqref="G17:K17"/>
+      <selection pane="bottomRight" activeCell="S15" sqref="S15:S26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12105,7 +12105,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12196,8 +12196,8 @@
       <c r="D4" t="s">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
-        <v>0</v>
+      <c r="E4">
+        <v>9000000</v>
       </c>
       <c r="F4">
         <v>3602.46</v>

</xml_diff>